<commit_message>
Pickup capacity constraints & pretty printing
</commit_message>
<xml_diff>
--- a/data/centres.xlsx
+++ b/data/centres.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\ubuntu\home\pierre\routage-du-coeur\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F1BFD4-581F-49ED-A09A-F47D53B24C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,6 +40,9 @@
     <t>Tonnage Surgelé (kg)</t>
   </si>
   <si>
+    <t>Semaine</t>
+  </si>
+  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -239,15 +236,13 @@
   </si>
   <si>
     <t>134, rue de la République, 31290 - VILLEFRANCHE DE LAURAGEAIS</t>
-  </si>
-  <si>
-    <t>Semaine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -258,7 +253,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -311,41 +306,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="12">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -356,10 +360,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -397,71 +401,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -489,7 +493,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -512,11 +516,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -525,13 +529,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -541,7 +545,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -550,7 +554,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -559,7 +563,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -567,10 +571,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -635,26 +639,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,29 +687,30 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>73</v>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5"/>
       <c r="F2" s="4">
         <v>3643</v>
       </c>
@@ -711,58 +720,63 @@
       <c r="H2" s="4">
         <v>366</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>43.639123300000001</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>43.6391233</v>
+      </c>
+      <c r="K2" s="7">
         <v>1.4356993</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="4">
         <v>115</v>
       </c>
       <c r="G3" s="4">
         <v>89</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>43.351893799999999</v>
-      </c>
-      <c r="K3" s="5">
+      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>43.3518938</v>
+      </c>
+      <c r="K3" s="7">
         <v>1.479144</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="4">
         <v>78</v>
       </c>
@@ -772,29 +786,30 @@
       <c r="H4" s="4">
         <v>35</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="6">
         <v>1</v>
       </c>
-      <c r="J4" s="5">
-        <v>42.791152699999998</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.58811159999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="7">
+        <v>42.7911527</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.5881116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="4">
         <v>482</v>
       </c>
@@ -804,29 +819,30 @@
       <c r="H5" s="4">
         <v>55</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="6">
         <v>1</v>
       </c>
-      <c r="J5" s="5">
-        <v>43.800681599999997</v>
-      </c>
-      <c r="K5" s="5">
-        <v>1.6040232999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="7">
+        <v>43.8006816</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1.6040233</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="4">
         <v>609</v>
       </c>
@@ -836,29 +852,30 @@
       <c r="H6" s="4">
         <v>86</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>43.646757299999997</v>
-      </c>
-      <c r="K6" s="5">
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>43.6467573</v>
+      </c>
+      <c r="K6" s="7">
         <v>1.3867645</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="4">
         <v>305</v>
       </c>
@@ -868,29 +885,30 @@
       <c r="H7" s="4">
         <v>23</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>43.297193399999998</v>
-      </c>
-      <c r="K7" s="5">
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>43.2971934</v>
+      </c>
+      <c r="K7" s="7">
         <v>1.2206374</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="4">
         <v>139</v>
       </c>
@@ -900,29 +918,30 @@
       <c r="H8" s="4">
         <v>11</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>43.210396299999999</v>
-      </c>
-      <c r="K8" s="5">
-        <v>1.1059543999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>43.2103963</v>
+      </c>
+      <c r="K8" s="7">
+        <v>1.1059544</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
+      <c r="C9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="4">
         <v>616</v>
       </c>
@@ -932,29 +951,30 @@
       <c r="H9" s="4">
         <v>86</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="6">
         <v>2</v>
       </c>
-      <c r="J9" s="5">
-        <v>43.534774800000001</v>
-      </c>
-      <c r="K9" s="5">
-        <v>1.3502449000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="7">
+        <v>43.5347748</v>
+      </c>
+      <c r="K9" s="7">
+        <v>1.3502449</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
+      <c r="C10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="4">
         <v>988</v>
       </c>
@@ -964,29 +984,30 @@
       <c r="H10" s="4">
         <v>94</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
-        <v>43.517648000000001</v>
-      </c>
-      <c r="K10" s="5">
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <v>43.517648</v>
+      </c>
+      <c r="K10" s="7">
         <v>1.5575128</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
+      <c r="C11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="5"/>
       <c r="F11" s="4">
         <v>102</v>
       </c>
@@ -996,29 +1017,30 @@
       <c r="H11" s="4">
         <v>26</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>43.684822500000003</v>
-      </c>
-      <c r="K11" s="5">
-        <v>1.4029818999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <v>43.6848225</v>
+      </c>
+      <c r="K11" s="7">
+        <v>1.4029819</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="D12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="5"/>
       <c r="F12" s="4">
         <v>448</v>
       </c>
@@ -1028,81 +1050,96 @@
       <c r="H12" s="4">
         <v>65</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="6">
         <v>1</v>
       </c>
-      <c r="J12" s="5">
-        <v>43.538938100000003</v>
-      </c>
-      <c r="K12" s="5">
-        <v>1.2351878999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="7">
+        <v>43.5389381</v>
+      </c>
+      <c r="K12" s="7">
+        <v>1.2351879</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13">
+      <c r="C13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4">
+        <v>448</v>
+      </c>
+      <c r="G13" s="4">
+        <v>249</v>
+      </c>
+      <c r="H13" s="4">
+        <v>65</v>
+      </c>
+      <c r="I13" s="6">
         <v>1</v>
       </c>
-      <c r="J13" s="5">
-        <v>43.838161100000001</v>
-      </c>
-      <c r="K13" s="5">
-        <v>1.3908275000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="7">
+        <v>43.8381611</v>
+      </c>
+      <c r="K13" s="7">
+        <v>1.3908275</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="5"/>
       <c r="F14" s="4">
         <v>78</v>
       </c>
       <c r="G14" s="4">
         <v>290</v>
       </c>
-      <c r="I14">
+      <c r="H14" s="8">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
         <v>1</v>
       </c>
-      <c r="J14" s="5">
-        <v>43.376576999999997</v>
-      </c>
-      <c r="K14" s="5">
+      <c r="J14" s="7">
+        <v>43.376577</v>
+      </c>
+      <c r="K14" s="7">
         <v>0.8372039</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
+      <c r="C15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="5"/>
       <c r="F15" s="4">
         <v>170</v>
       </c>
@@ -1112,29 +1149,30 @@
       <c r="H15" s="4">
         <v>28</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>43.599054000000002</v>
-      </c>
-      <c r="K15" s="5">
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <v>43.599054</v>
+      </c>
+      <c r="K15" s="7">
         <v>1.236362</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D16" t="s">
-        <v>21</v>
-      </c>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="5"/>
       <c r="F16" s="4">
         <v>147</v>
       </c>
@@ -1144,29 +1182,30 @@
       <c r="H16" s="4">
         <v>27</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="6">
         <v>2</v>
       </c>
-      <c r="J16" s="5">
-        <v>43.667095499999988</v>
-      </c>
-      <c r="K16" s="5">
-        <v>1.1934514000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="7">
+        <v>43.66709549999999</v>
+      </c>
+      <c r="K16" s="7">
+        <v>1.1934514</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
+      <c r="C17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="5"/>
       <c r="F17" s="4">
         <v>85</v>
       </c>
@@ -1176,29 +1215,30 @@
       <c r="H17" s="4">
         <v>6</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>43.084641300000001</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0.56264809999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I17" s="6">
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <v>43.0846413</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0.5626481</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
+      <c r="C18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="5"/>
       <c r="F18" s="4">
         <v>253</v>
       </c>
@@ -1208,29 +1248,30 @@
       <c r="H18" s="4">
         <v>67</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <v>43.478209000000007</v>
-      </c>
-      <c r="K18" s="5">
-        <v>1.3417749999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="6">
+        <v>0</v>
+      </c>
+      <c r="J18" s="7">
+        <v>43.47820900000001</v>
+      </c>
+      <c r="K18" s="7">
+        <v>1.341775</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
+      <c r="C19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="4">
         <v>1411</v>
       </c>
@@ -1240,29 +1281,30 @@
       <c r="H19" s="4">
         <v>273</v>
       </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <v>43.621826499999997</v>
-      </c>
-      <c r="K19" s="5">
+      <c r="I19" s="6">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <v>43.6218265</v>
+      </c>
+      <c r="K19" s="7">
         <v>1.2918542</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D20" t="s">
-        <v>36</v>
-      </c>
+      <c r="C20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="4">
         <v>219</v>
       </c>
@@ -1272,29 +1314,30 @@
       <c r="H20" s="4">
         <v>27</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5">
-        <v>43.567515999999998</v>
-      </c>
-      <c r="K20" s="5">
-        <v>1.3065979000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="6">
+        <v>0</v>
+      </c>
+      <c r="J20" s="7">
+        <v>43.567516</v>
+      </c>
+      <c r="K20" s="7">
+        <v>1.3065979</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
+      <c r="C21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="4">
         <v>635</v>
       </c>
@@ -1304,29 +1347,30 @@
       <c r="H21" s="4">
         <v>89</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <v>43.541869599999998</v>
-      </c>
-      <c r="K21" s="5">
-        <v>1.4085209000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I21" s="6">
+        <v>0</v>
+      </c>
+      <c r="J21" s="7">
+        <v>43.5418696</v>
+      </c>
+      <c r="K21" s="7">
+        <v>1.4085209</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
+      <c r="C22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="5"/>
       <c r="F22" s="4">
         <v>248</v>
       </c>
@@ -1336,81 +1380,96 @@
       <c r="H22" s="4">
         <v>63</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22" s="5">
-        <v>43.456546499999988</v>
-      </c>
-      <c r="K22" s="5">
-        <v>2.0037020999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="6">
+        <v>0</v>
+      </c>
+      <c r="J22" s="7">
+        <v>43.45654649999999</v>
+      </c>
+      <c r="K22" s="7">
+        <v>2.0037021</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23">
+      <c r="C23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="4">
+        <v>285</v>
+      </c>
+      <c r="G23" s="4">
+        <v>259</v>
+      </c>
+      <c r="H23" s="4">
+        <v>55</v>
+      </c>
+      <c r="I23" s="6">
         <v>2</v>
       </c>
-      <c r="J23" s="5">
-        <v>43.413303800000001</v>
-      </c>
-      <c r="K23" s="5">
-        <v>1.1190481999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="7">
+        <v>43.4133038</v>
+      </c>
+      <c r="K23" s="7">
+        <v>1.1190482</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D24" t="s">
-        <v>18</v>
-      </c>
+      <c r="C24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="5"/>
       <c r="F24" s="4">
         <v>406</v>
       </c>
       <c r="G24" s="4">
         <v>326</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24" s="5">
-        <v>43.106198999999997</v>
-      </c>
-      <c r="K24" s="5">
-        <v>0.72626089999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="8">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0</v>
+      </c>
+      <c r="J24" s="7">
+        <v>43.106199</v>
+      </c>
+      <c r="K24" s="7">
+        <v>0.7262609</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="5"/>
       <c r="F25" s="4">
         <v>285</v>
       </c>
@@ -1420,29 +1479,30 @@
       <c r="H25" s="4">
         <v>55</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25" s="5">
-        <v>43.083461200000002</v>
-      </c>
-      <c r="K25" s="5">
-        <v>0.94692469999999995</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="6">
+        <v>0</v>
+      </c>
+      <c r="J25" s="7">
+        <v>43.0834612</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0.9469247</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
+      <c r="C26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="5"/>
       <c r="F26" s="4">
         <v>613</v>
       </c>
@@ -1452,29 +1512,30 @@
       <c r="H26" s="4">
         <v>152</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26" s="5">
-        <v>43.603527500000013</v>
-      </c>
-      <c r="K26" s="5">
-        <v>1.4076352999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="6">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7">
+        <v>43.60352750000001</v>
+      </c>
+      <c r="K26" s="7">
+        <v>1.4076353</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
+      <c r="C27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="4">
         <v>4289</v>
       </c>
@@ -1484,29 +1545,30 @@
       <c r="H27" s="4">
         <v>172</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
-        <v>43.565138900000008</v>
-      </c>
-      <c r="K27" s="5">
-        <v>1.5106987999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I27" s="6">
+        <v>0</v>
+      </c>
+      <c r="J27" s="7">
+        <v>43.56513890000001</v>
+      </c>
+      <c r="K27" s="7">
+        <v>1.5106988</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D28" t="s">
-        <v>15</v>
-      </c>
+      <c r="C28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="5"/>
       <c r="F28" s="4">
         <v>1859</v>
       </c>
@@ -1516,29 +1578,30 @@
       <c r="H28" s="4">
         <v>317</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28" s="5">
-        <v>43.592840799999998</v>
-      </c>
-      <c r="K28" s="5">
-        <v>1.4113336000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="6">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7">
+        <v>43.5928408</v>
+      </c>
+      <c r="K28" s="7">
+        <v>1.4113336</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="4">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D29" t="s">
-        <v>21</v>
-      </c>
+      <c r="C29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="5"/>
       <c r="F29" s="4">
         <v>592</v>
       </c>
@@ -1548,29 +1611,30 @@
       <c r="H29" s="4">
         <v>26</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29" s="5">
-        <v>43.577175099999998</v>
-      </c>
-      <c r="K29" s="5">
+      <c r="I29" s="6">
+        <v>0</v>
+      </c>
+      <c r="J29" s="7">
+        <v>43.5771751</v>
+      </c>
+      <c r="K29" s="7">
         <v>1.3259272</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D30" t="s">
-        <v>15</v>
-      </c>
+      <c r="C30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="5"/>
       <c r="F30" s="4">
         <v>79</v>
       </c>
@@ -1580,13 +1644,13 @@
       <c r="H30" s="4">
         <v>29</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30" s="5">
-        <v>43.401530000000001</v>
-      </c>
-      <c r="K30" s="5">
+      <c r="I30" s="6">
+        <v>0</v>
+      </c>
+      <c r="J30" s="7">
+        <v>43.40153</v>
+      </c>
+      <c r="K30" s="7">
         <v>1.7137495</v>
       </c>
     </row>

</xml_diff>

<commit_message>
performance improvement + demi palettes
</commit_message>
<xml_diff>
--- a/data/centres.xlsx
+++ b/data/centres.xlsx
@@ -306,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,13 +323,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -649,20 +646,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -720,13 +717,13 @@
       <c r="H2" s="4">
         <v>366</v>
       </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="7">
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
         <v>43.6391233</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>1.4356993</v>
       </c>
     </row>
@@ -750,16 +747,16 @@
       <c r="G3" s="4">
         <v>89</v>
       </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="7">
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
         <v>43.3518938</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>1.479144</v>
       </c>
     </row>
@@ -786,13 +783,13 @@
       <c r="H4" s="4">
         <v>35</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="4">
         <v>1</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>42.7911527</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>0.5881116</v>
       </c>
     </row>
@@ -819,13 +816,13 @@
       <c r="H5" s="4">
         <v>55</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="4">
         <v>1</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <v>43.8006816</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>1.6040233</v>
       </c>
     </row>
@@ -852,13 +849,13 @@
       <c r="H6" s="4">
         <v>86</v>
       </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7">
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
         <v>43.6467573</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>1.3867645</v>
       </c>
     </row>
@@ -885,13 +882,13 @@
       <c r="H7" s="4">
         <v>23</v>
       </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7">
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
         <v>43.2971934</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>1.2206374</v>
       </c>
     </row>
@@ -918,13 +915,13 @@
       <c r="H8" s="4">
         <v>11</v>
       </c>
-      <c r="I8" s="6">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
         <v>43.2103963</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>1.1059544</v>
       </c>
     </row>
@@ -951,13 +948,13 @@
       <c r="H9" s="4">
         <v>86</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="4">
         <v>2</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <v>43.5347748</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>1.3502449</v>
       </c>
     </row>
@@ -984,13 +981,13 @@
       <c r="H10" s="4">
         <v>94</v>
       </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="7">
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
         <v>43.517648</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <v>1.5575128</v>
       </c>
     </row>
@@ -1017,13 +1014,13 @@
       <c r="H11" s="4">
         <v>26</v>
       </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7">
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
         <v>43.6848225</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>1.4029819</v>
       </c>
     </row>
@@ -1050,13 +1047,13 @@
       <c r="H12" s="4">
         <v>65</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="4">
         <v>1</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>43.5389381</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>1.2351879</v>
       </c>
     </row>
@@ -1083,13 +1080,13 @@
       <c r="H13" s="4">
         <v>65</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="4">
         <v>1</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="6">
         <v>43.8381611</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <v>1.3908275</v>
       </c>
     </row>
@@ -1113,16 +1110,16 @@
       <c r="G14" s="4">
         <v>290</v>
       </c>
-      <c r="H14" s="8">
-        <v>0</v>
-      </c>
-      <c r="I14" s="6">
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
         <v>1</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="6">
         <v>43.376577</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <v>0.8372039</v>
       </c>
     </row>
@@ -1149,13 +1146,13 @@
       <c r="H15" s="4">
         <v>28</v>
       </c>
-      <c r="I15" s="6">
-        <v>0</v>
-      </c>
-      <c r="J15" s="7">
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="6">
         <v>43.599054</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <v>1.236362</v>
       </c>
     </row>
@@ -1182,13 +1179,13 @@
       <c r="H16" s="4">
         <v>27</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="4">
         <v>2</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="6">
         <v>43.66709549999999</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <v>1.1934514</v>
       </c>
     </row>
@@ -1215,13 +1212,13 @@
       <c r="H17" s="4">
         <v>6</v>
       </c>
-      <c r="I17" s="6">
-        <v>0</v>
-      </c>
-      <c r="J17" s="7">
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="6">
         <v>43.0846413</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <v>0.5626481</v>
       </c>
     </row>
@@ -1248,13 +1245,13 @@
       <c r="H18" s="4">
         <v>67</v>
       </c>
-      <c r="I18" s="6">
-        <v>0</v>
-      </c>
-      <c r="J18" s="7">
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="6">
         <v>43.47820900000001</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="6">
         <v>1.341775</v>
       </c>
     </row>
@@ -1281,13 +1278,13 @@
       <c r="H19" s="4">
         <v>273</v>
       </c>
-      <c r="I19" s="6">
-        <v>0</v>
-      </c>
-      <c r="J19" s="7">
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="6">
         <v>43.6218265</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="6">
         <v>1.2918542</v>
       </c>
     </row>
@@ -1314,13 +1311,13 @@
       <c r="H20" s="4">
         <v>27</v>
       </c>
-      <c r="I20" s="6">
-        <v>0</v>
-      </c>
-      <c r="J20" s="7">
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="6">
         <v>43.567516</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="6">
         <v>1.3065979</v>
       </c>
     </row>
@@ -1347,13 +1344,13 @@
       <c r="H21" s="4">
         <v>89</v>
       </c>
-      <c r="I21" s="6">
-        <v>0</v>
-      </c>
-      <c r="J21" s="7">
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="6">
         <v>43.5418696</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <v>1.4085209</v>
       </c>
     </row>
@@ -1380,13 +1377,13 @@
       <c r="H22" s="4">
         <v>63</v>
       </c>
-      <c r="I22" s="6">
-        <v>0</v>
-      </c>
-      <c r="J22" s="7">
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="6">
         <v>43.45654649999999</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="6">
         <v>2.0037021</v>
       </c>
     </row>
@@ -1413,13 +1410,13 @@
       <c r="H23" s="4">
         <v>55</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="4">
         <v>2</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="6">
         <v>43.4133038</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="6">
         <v>1.1190482</v>
       </c>
     </row>
@@ -1443,16 +1440,16 @@
       <c r="G24" s="4">
         <v>326</v>
       </c>
-      <c r="H24" s="8">
-        <v>0</v>
-      </c>
-      <c r="I24" s="6">
-        <v>0</v>
-      </c>
-      <c r="J24" s="7">
+      <c r="H24" s="7">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="6">
         <v>43.106199</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="6">
         <v>0.7262609</v>
       </c>
     </row>
@@ -1479,13 +1476,13 @@
       <c r="H25" s="4">
         <v>55</v>
       </c>
-      <c r="I25" s="6">
-        <v>0</v>
-      </c>
-      <c r="J25" s="7">
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="6">
         <v>43.0834612</v>
       </c>
-      <c r="K25" s="7">
+      <c r="K25" s="6">
         <v>0.9469247</v>
       </c>
     </row>
@@ -1512,13 +1509,13 @@
       <c r="H26" s="4">
         <v>152</v>
       </c>
-      <c r="I26" s="6">
-        <v>0</v>
-      </c>
-      <c r="J26" s="7">
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="6">
         <v>43.60352750000001</v>
       </c>
-      <c r="K26" s="7">
+      <c r="K26" s="6">
         <v>1.4076353</v>
       </c>
     </row>
@@ -1545,13 +1542,13 @@
       <c r="H27" s="4">
         <v>172</v>
       </c>
-      <c r="I27" s="6">
-        <v>0</v>
-      </c>
-      <c r="J27" s="7">
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="6">
         <v>43.56513890000001</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="6">
         <v>1.5106988</v>
       </c>
     </row>
@@ -1578,13 +1575,13 @@
       <c r="H28" s="4">
         <v>317</v>
       </c>
-      <c r="I28" s="6">
-        <v>0</v>
-      </c>
-      <c r="J28" s="7">
+      <c r="I28" s="4">
+        <v>0</v>
+      </c>
+      <c r="J28" s="6">
         <v>43.5928408</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="6">
         <v>1.4113336</v>
       </c>
     </row>
@@ -1611,13 +1608,13 @@
       <c r="H29" s="4">
         <v>26</v>
       </c>
-      <c r="I29" s="6">
-        <v>0</v>
-      </c>
-      <c r="J29" s="7">
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="6">
         <v>43.5771751</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="6">
         <v>1.3259272</v>
       </c>
     </row>
@@ -1644,13 +1641,13 @@
       <c r="H30" s="4">
         <v>29</v>
       </c>
-      <c r="I30" s="6">
-        <v>0</v>
-      </c>
-      <c r="J30" s="7">
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="6">
         <v>43.40153</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="6">
         <v>1.7137495</v>
       </c>
     </row>

</xml_diff>

<commit_message>
performance improvements, tour duration limit, week assignment benchmarks
</commit_message>
<xml_diff>
--- a/data/centres.xlsx
+++ b/data/centres.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\ubuntu\home\pierre\routage-du-coeur\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0792E5-508F-475F-AA90-9131717307C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -212,6 +206,9 @@
   </si>
   <si>
     <t>29 Rue du 19 Mars 1962, 31820 Pibrac</t>
+  </si>
+  <si>
+    <t>Lundi, Jeudi</t>
   </si>
   <si>
     <t>Plaisance du Touch</t>
@@ -310,7 +307,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,44 +377,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="11">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -427,10 +428,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -468,71 +469,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -560,7 +561,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -583,11 +584,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -596,13 +597,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -612,7 +613,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -621,7 +622,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -630,7 +631,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -638,10 +639,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -706,27 +707,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="32.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,19 +773,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="E2" s="6"/>
       <c r="F2" s="5">
         <v>3643</v>
       </c>
@@ -792,26 +799,29 @@
       <c r="I2" s="5">
         <v>0</v>
       </c>
-      <c r="J2" s="6">
-        <v>43.639123300000001</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="J2" s="7">
+        <v>43.6391233</v>
+      </c>
+      <c r="K2" s="7">
         <v>1.4356993</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="E3" s="6"/>
       <c r="F3" s="5">
         <v>115</v>
       </c>
@@ -824,32 +834,33 @@
       <c r="I3" s="5">
         <v>0</v>
       </c>
-      <c r="J3" s="6">
-        <v>43.351893799999999</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="J3" s="7">
+        <v>43.3518938</v>
+      </c>
+      <c r="K3" s="7">
         <v>1.479144</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="E4" s="6"/>
       <c r="F4" s="5">
         <v>78</v>
       </c>
@@ -862,32 +873,33 @@
       <c r="I4" s="5">
         <v>1</v>
       </c>
-      <c r="J4" s="6">
-        <v>42.791152699999998</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0.58811159999999996</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="J4" s="7">
+        <v>42.7911527</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.5881116</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="E5" s="6"/>
       <c r="F5" s="5">
         <v>482</v>
       </c>
@@ -900,32 +912,33 @@
       <c r="I5" s="5">
         <v>1</v>
       </c>
-      <c r="J5" s="6">
-        <v>43.800681599999997</v>
-      </c>
-      <c r="K5" s="6">
-        <v>1.6040232999999999</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="J5" s="7">
+        <v>43.8006816</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1.6040233</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="5">
         <v>609</v>
       </c>
@@ -938,32 +951,33 @@
       <c r="I6" s="5">
         <v>0</v>
       </c>
-      <c r="J6" s="6">
-        <v>43.646757299999997</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="J6" s="7">
+        <v>43.6467573</v>
+      </c>
+      <c r="K6" s="7">
         <v>1.3867645</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="5">
         <v>305</v>
       </c>
@@ -976,32 +990,33 @@
       <c r="I7" s="5">
         <v>0</v>
       </c>
-      <c r="J7" s="6">
-        <v>43.297193399999998</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="J7" s="7">
+        <v>43.2971934</v>
+      </c>
+      <c r="K7" s="7">
         <v>1.2206374</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="E8" s="6"/>
       <c r="F8" s="5">
         <v>139</v>
       </c>
@@ -1014,32 +1029,33 @@
       <c r="I8" s="5">
         <v>0</v>
       </c>
-      <c r="J8" s="6">
-        <v>43.210396299999999</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1.1059543999999999</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="J8" s="7">
+        <v>43.2103963</v>
+      </c>
+      <c r="K8" s="7">
+        <v>1.1059544</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="E9" s="6"/>
       <c r="F9" s="5">
         <v>616</v>
       </c>
@@ -1052,32 +1068,33 @@
       <c r="I9" s="5">
         <v>2</v>
       </c>
-      <c r="J9" s="6">
-        <v>43.534774800000001</v>
-      </c>
-      <c r="K9" s="6">
-        <v>1.3502449000000001</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="J9" s="7">
+        <v>43.5347748</v>
+      </c>
+      <c r="K9" s="7">
+        <v>1.3502449</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="E10" s="6"/>
       <c r="F10" s="5">
         <v>988</v>
       </c>
@@ -1090,32 +1107,33 @@
       <c r="I10" s="5">
         <v>0</v>
       </c>
-      <c r="J10" s="6">
-        <v>43.517648000000001</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="J10" s="7">
+        <v>43.517648</v>
+      </c>
+      <c r="K10" s="7">
         <v>1.5575128</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="E11" s="6"/>
       <c r="F11" s="5">
         <v>102</v>
       </c>
@@ -1128,32 +1146,33 @@
       <c r="I11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="6">
-        <v>43.684822500000003</v>
-      </c>
-      <c r="K11" s="6">
-        <v>1.4029818999999999</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="J11" s="7">
+        <v>43.6848225</v>
+      </c>
+      <c r="K11" s="7">
+        <v>1.4029819</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="E12" s="6"/>
       <c r="F12" s="5">
         <v>448</v>
       </c>
@@ -1166,32 +1185,33 @@
       <c r="I12" s="5">
         <v>1</v>
       </c>
-      <c r="J12" s="6">
-        <v>43.538938100000003</v>
-      </c>
-      <c r="K12" s="6">
-        <v>1.2351878999999999</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="J12" s="7">
+        <v>43.5389381</v>
+      </c>
+      <c r="K12" s="7">
+        <v>1.2351879</v>
+      </c>
+      <c r="L12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="E13" s="6"/>
       <c r="F13" s="5">
         <v>448</v>
       </c>
@@ -1204,32 +1224,33 @@
       <c r="I13" s="5">
         <v>1</v>
       </c>
-      <c r="J13" s="6">
-        <v>43.838161100000001</v>
-      </c>
-      <c r="K13" s="6">
-        <v>1.3908275000000001</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="J13" s="7">
+        <v>43.8381611</v>
+      </c>
+      <c r="K13" s="7">
+        <v>1.3908275</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="E14" s="6"/>
       <c r="F14" s="5">
         <v>78</v>
       </c>
@@ -1242,32 +1263,33 @@
       <c r="I14" s="5">
         <v>1</v>
       </c>
-      <c r="J14" s="6">
-        <v>43.376576999999997</v>
-      </c>
-      <c r="K14" s="6">
+      <c r="J14" s="7">
+        <v>43.376577</v>
+      </c>
+      <c r="K14" s="7">
         <v>0.8372039</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="E15" s="6"/>
       <c r="F15" s="5">
         <v>170</v>
       </c>
@@ -1280,32 +1302,33 @@
       <c r="I15" s="5">
         <v>0</v>
       </c>
-      <c r="J15" s="6">
-        <v>43.599054000000002</v>
-      </c>
-      <c r="K15" s="6">
+      <c r="J15" s="7">
+        <v>43.599054</v>
+      </c>
+      <c r="K15" s="7">
         <v>1.236362</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="5">
         <v>147</v>
       </c>
@@ -1318,32 +1341,33 @@
       <c r="I16" s="5">
         <v>2</v>
       </c>
-      <c r="J16" s="6">
-        <v>43.667095499999988</v>
-      </c>
-      <c r="K16" s="6">
-        <v>1.1934514000000001</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="J16" s="7">
+        <v>43.66709549999999</v>
+      </c>
+      <c r="K16" s="7">
+        <v>1.1934514</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="E17" s="6"/>
       <c r="F17" s="5">
         <v>85</v>
       </c>
@@ -1356,32 +1380,33 @@
       <c r="I17" s="5">
         <v>0</v>
       </c>
-      <c r="J17" s="6">
-        <v>43.084641300000001</v>
-      </c>
-      <c r="K17" s="6">
-        <v>0.56264809999999998</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="J17" s="7">
+        <v>43.0846413</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0.5626481</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="5">
         <v>253</v>
       </c>
@@ -1394,32 +1419,33 @@
       <c r="I18" s="5">
         <v>0</v>
       </c>
-      <c r="J18" s="6">
-        <v>43.478209000000007</v>
-      </c>
-      <c r="K18" s="6">
-        <v>1.3417749999999999</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="J18" s="7">
+        <v>43.47820900000001</v>
+      </c>
+      <c r="K18" s="7">
+        <v>1.341775</v>
+      </c>
+      <c r="L18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="E19" s="6"/>
       <c r="F19" s="5">
         <v>1411</v>
       </c>
@@ -1432,32 +1458,33 @@
       <c r="I19" s="5">
         <v>0</v>
       </c>
-      <c r="J19" s="6">
-        <v>43.621826499999997</v>
-      </c>
-      <c r="K19" s="6">
+      <c r="J19" s="7">
+        <v>43.6218265</v>
+      </c>
+      <c r="K19" s="7">
         <v>1.2918542</v>
       </c>
-      <c r="L19" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="5">
         <v>219</v>
       </c>
@@ -1470,32 +1497,33 @@
       <c r="I20" s="5">
         <v>0</v>
       </c>
-      <c r="J20" s="6">
-        <v>43.567515999999998</v>
-      </c>
-      <c r="K20" s="6">
-        <v>1.3065979000000001</v>
-      </c>
-      <c r="L20" t="s">
-        <v>66</v>
-      </c>
-      <c r="M20" t="s">
+      <c r="J20" s="7">
+        <v>43.567516</v>
+      </c>
+      <c r="K20" s="7">
+        <v>1.3065979</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="E21" s="6"/>
       <c r="F21" s="5">
         <v>635</v>
       </c>
@@ -1508,32 +1536,33 @@
       <c r="I21" s="5">
         <v>0</v>
       </c>
-      <c r="J21" s="6">
-        <v>43.541869599999998</v>
-      </c>
-      <c r="K21" s="6">
-        <v>1.4085209000000001</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="J21" s="7">
+        <v>43.5418696</v>
+      </c>
+      <c r="K21" s="7">
+        <v>1.4085209</v>
+      </c>
+      <c r="L21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="E22" s="6"/>
       <c r="F22" s="5">
         <v>248</v>
       </c>
@@ -1546,32 +1575,33 @@
       <c r="I22" s="5">
         <v>0</v>
       </c>
-      <c r="J22" s="6">
-        <v>43.456546499999988</v>
-      </c>
-      <c r="K22" s="6">
-        <v>2.0037020999999999</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="J22" s="7">
+        <v>43.45654649999999</v>
+      </c>
+      <c r="K22" s="7">
+        <v>2.0037021</v>
+      </c>
+      <c r="L22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="5">
         <v>285</v>
       </c>
@@ -1584,32 +1614,33 @@
       <c r="I23" s="5">
         <v>2</v>
       </c>
-      <c r="J23" s="6">
-        <v>43.413303800000001</v>
-      </c>
-      <c r="K23" s="6">
-        <v>1.1190481999999999</v>
-      </c>
-      <c r="L23" t="s">
-        <v>73</v>
-      </c>
-      <c r="M23" t="s">
+      <c r="J23" s="7">
+        <v>43.4133038</v>
+      </c>
+      <c r="K23" s="7">
+        <v>1.1190482</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M23" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24" s="6" t="s">
         <v>76</v>
       </c>
+      <c r="D24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="5">
         <v>406</v>
       </c>
@@ -1622,32 +1653,33 @@
       <c r="I24" s="5">
         <v>0</v>
       </c>
-      <c r="J24" s="6">
-        <v>43.106198999999997</v>
-      </c>
-      <c r="K24" s="6">
-        <v>0.72626089999999999</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="J24" s="7">
+        <v>43.106199</v>
+      </c>
+      <c r="K24" s="7">
+        <v>0.7262609</v>
+      </c>
+      <c r="L24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="5">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25" s="6" t="s">
         <v>79</v>
       </c>
+      <c r="D25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="5">
         <v>285</v>
       </c>
@@ -1660,32 +1692,33 @@
       <c r="I25" s="5">
         <v>0</v>
       </c>
-      <c r="J25" s="6">
-        <v>43.083461200000002</v>
-      </c>
-      <c r="K25" s="6">
-        <v>0.94692469999999995</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="J25" s="7">
+        <v>43.0834612</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0.9469247</v>
+      </c>
+      <c r="L25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="E26" s="6"/>
       <c r="F26" s="5">
         <v>613</v>
       </c>
@@ -1698,32 +1731,33 @@
       <c r="I26" s="5">
         <v>0</v>
       </c>
-      <c r="J26" s="6">
-        <v>43.603527500000013</v>
-      </c>
-      <c r="K26" s="6">
-        <v>1.4076352999999999</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="J26" s="7">
+        <v>43.60352750000001</v>
+      </c>
+      <c r="K26" s="7">
+        <v>1.4076353</v>
+      </c>
+      <c r="L26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="5">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C27" s="6" t="s">
         <v>84</v>
       </c>
+      <c r="D27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="6"/>
       <c r="F27" s="5">
         <v>4289</v>
       </c>
@@ -1736,32 +1770,33 @@
       <c r="I27" s="5">
         <v>0</v>
       </c>
-      <c r="J27" s="6">
-        <v>43.565138900000008</v>
-      </c>
-      <c r="K27" s="6">
-        <v>1.5106987999999999</v>
-      </c>
-      <c r="L27" t="s">
-        <v>85</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="J27" s="7">
+        <v>43.56513890000001</v>
+      </c>
+      <c r="K27" s="7">
+        <v>1.5106988</v>
+      </c>
+      <c r="L27" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="5">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="E28" s="6"/>
       <c r="F28" s="5">
         <v>1859</v>
       </c>
@@ -1774,32 +1809,33 @@
       <c r="I28" s="5">
         <v>0</v>
       </c>
-      <c r="J28" s="6">
-        <v>43.592840799999998</v>
-      </c>
-      <c r="K28" s="6">
-        <v>1.4113336000000001</v>
-      </c>
-      <c r="L28" t="s">
-        <v>89</v>
-      </c>
-      <c r="M28" t="s">
+      <c r="J28" s="7">
+        <v>43.5928408</v>
+      </c>
+      <c r="K28" s="7">
+        <v>1.4113336</v>
+      </c>
+      <c r="L28" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M28" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="5">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C29" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="E29" s="6"/>
       <c r="F29" s="5">
         <v>592</v>
       </c>
@@ -1812,32 +1848,33 @@
       <c r="I29" s="5">
         <v>0</v>
       </c>
-      <c r="J29" s="6">
-        <v>43.577175099999998</v>
-      </c>
-      <c r="K29" s="6">
+      <c r="J29" s="7">
+        <v>43.5771751</v>
+      </c>
+      <c r="K29" s="7">
         <v>1.3259272</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M29" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="5">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="E30" s="6"/>
       <c r="F30" s="5">
         <v>79</v>
       </c>
@@ -1850,16 +1887,16 @@
       <c r="I30" s="5">
         <v>0</v>
       </c>
-      <c r="J30" s="6">
-        <v>43.401530000000001</v>
-      </c>
-      <c r="K30" s="6">
+      <c r="J30" s="7">
+        <v>43.40153</v>
+      </c>
+      <c r="K30" s="7">
         <v>1.7137495</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M30" s="6" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added some options for handling demand uncertainty + study of bidaily delivery
</commit_message>
<xml_diff>
--- a/data/centres.xlsx
+++ b/data/centres.xlsx
@@ -829,7 +829,7 @@
         <v>89</v>
       </c>
       <c r="H3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="5">
         <v>0</v>
@@ -1258,7 +1258,7 @@
         <v>290</v>
       </c>
       <c r="H14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="5">
         <v>1</v>
@@ -1648,7 +1648,7 @@
         <v>326</v>
       </c>
       <c r="H24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
new constraints & data adjustments
</commit_message>
<xml_diff>
--- a/data/centres.xlsx
+++ b/data/centres.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>15 Avenue du Comminges, 31260 - Mane</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Toulouse/Grande-Bretagne(Casselardit)</t>
@@ -732,7 +729,7 @@
     <col min="13" max="13" style="9" width="32.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,7 +826,7 @@
         <v>89</v>
       </c>
       <c r="H3" s="5">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="I3" s="5">
         <v>0</v>
@@ -985,7 +982,7 @@
         <v>126</v>
       </c>
       <c r="H7" s="5">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="I7" s="5">
         <v>0</v>
@@ -1024,7 +1021,7 @@
         <v>100</v>
       </c>
       <c r="H8" s="5">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="I8" s="5">
         <v>0</v>
@@ -1141,7 +1138,7 @@
         <v>164</v>
       </c>
       <c r="H11" s="5">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I11" s="5">
         <v>0</v>
@@ -1258,7 +1255,7 @@
         <v>290</v>
       </c>
       <c r="H14" s="5">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="I14" s="5">
         <v>1</v>
@@ -1297,7 +1294,7 @@
         <v>105</v>
       </c>
       <c r="H15" s="5">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I15" s="5">
         <v>0</v>
@@ -1336,7 +1333,7 @@
         <v>174</v>
       </c>
       <c r="H16" s="5">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I16" s="5">
         <v>2</v>
@@ -1375,7 +1372,7 @@
         <v>92</v>
       </c>
       <c r="H17" s="5">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="I17" s="5">
         <v>0</v>
@@ -1492,7 +1489,7 @@
         <v>86</v>
       </c>
       <c r="H20" s="5">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I20" s="5">
         <v>0</v>
@@ -1648,7 +1645,7 @@
         <v>326</v>
       </c>
       <c r="H24" s="5">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I24" s="5">
         <v>0</v>
@@ -1677,7 +1674,7 @@
         <v>79</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="5">
@@ -1710,10 +1707,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>23</v>
@@ -1749,13 +1746,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="5">
@@ -1777,10 +1774,10 @@
         <v>1.5106988</v>
       </c>
       <c r="L27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="M27" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
@@ -1788,10 +1785,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>20</v>
@@ -1816,10 +1813,10 @@
         <v>1.4113336</v>
       </c>
       <c r="L28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M28" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
@@ -1827,10 +1824,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>25</v>
@@ -1843,7 +1840,7 @@
         <v>353</v>
       </c>
       <c r="H29" s="5">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I29" s="5">
         <v>0</v>
@@ -1866,10 +1863,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>20</v>
@@ -1882,7 +1879,7 @@
         <v>170</v>
       </c>
       <c r="H30" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I30" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
tour durations in txt files & adjustments
</commit_message>
<xml_diff>
--- a/data/centres.xlsx
+++ b/data/centres.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="94">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -271,19 +271,16 @@
     <t>Lundi/Mardi/Mercredi</t>
   </si>
   <si>
-    <t>Lundi, Mardi, Mercredi, Jeudi, Vendredi</t>
-  </si>
-  <si>
-    <t>Lundi,Mardi,Mercredi,Jeudi,Vendredi (?)</t>
+    <t>Lundi, Mardi, Mercredi, Vendredi</t>
+  </si>
+  <si>
+    <t>Lundi,Mardi,Mercredi,Vendredi (?)</t>
   </si>
   <si>
     <t>Toulouse/Negogousses(Les Arenes)</t>
   </si>
   <si>
     <t>63 Rue de Negogousses, 31100 - Toulouse</t>
-  </si>
-  <si>
-    <t>Lundi, Mardi, Mercredi, Vendredi</t>
   </si>
   <si>
     <t>Lundi,Vendredi</t>
@@ -1813,10 +1810,10 @@
         <v>1.4113336</v>
       </c>
       <c r="L28" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="M28" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
@@ -1824,10 +1821,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>25</v>
@@ -1863,10 +1860,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>20</v>

</xml_diff>